<commit_message>
Added compare (flag) substitutions to LUT
</commit_message>
<xml_diff>
--- a/res/sub_table.xlsx
+++ b/res/sub_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="196">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -382,6 +382,14 @@
   </si>
   <si>
     <t xml:space="preserve">l.nop K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.nop K
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.nop K
+l.movhi r0,0</t>
   </si>
   <si>
     <t xml:space="preserve">l.or rD,rA,rB</t>
@@ -456,61 +464,143 @@
     <t xml:space="preserve">l.sfeq rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfeq rA,rB
+l.ff1 r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfeqi rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.xori r0,r0,I
+l.sfeq rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfges rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfles rB,rA</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfgesi rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.xori r0,r0,I
+l.sfges rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfgeu rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfleu rB,rA</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfgeui rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.ori r0,r0,I
+l.sfgeu rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfgts rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sflts rB,rA</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfgtsi rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.xori r0,r0,I
+l.sfgts rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfgtu rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfltu rB,rA</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfgtui rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.ori r0,r0,I
+l.sfgtu rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfles rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfges rB,rA</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sflesi rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.xori r0,r0,I
+l.sfles rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfleu rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfgeu rB,rA</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfleui rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.ori r0,r0,I
+l.sfleu rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sflts rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfgts rB,rA</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfltsi rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.xori r0,r0,I
+l.sflts rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfltu rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfgtu rB,rA</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfltui rA,I</t>
   </si>
   <si>
+    <t xml:space="preserve">l.ori r0,r0,I
+l.sfltu rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfne rA,rB</t>
   </si>
   <si>
+    <t xml:space="preserve">l.sfne rA,rB
+l.ff1 r0,r0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.sfnei rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.xori r0,r0,I
+l.sfne rA,r0
+l.xor r0,r0,r0</t>
   </si>
   <si>
     <t xml:space="preserve">l.sh I(rA),rB</t>
@@ -879,8 +969,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C95" activeCellId="0" sqref="C95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B71" activeCellId="0" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1466,21 +1556,27 @@
       <c r="C55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D56" s="5"/>
+      <c r="B56" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="5"/>
@@ -1488,19 +1584,19 @@
     </row>
     <row r="58" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="3"/>
@@ -1508,281 +1604,331 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
+    <row r="65" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="0"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" s="0"/>
       <c r="E66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B67" s="3"/>
+      <c r="A67" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" s="0"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C68" s="0"/>
       <c r="E68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
+      <c r="A69" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="0"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" s="0"/>
       <c r="E70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8" t="s">
-        <v>124</v>
-      </c>
+      <c r="A71" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="0"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="0"/>
       <c r="E72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8" t="s">
-        <v>126</v>
-      </c>
+      <c r="A73" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="0"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C74" s="0"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C75" s="3"/>
+      <c r="A75" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" s="0"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" s="0"/>
       <c r="E76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B77" s="3"/>
+      <c r="A77" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C77" s="0"/>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C78" s="0"/>
       <c r="E78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8" t="s">
-        <v>132</v>
-      </c>
+      <c r="A79" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C79" s="0"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
+    <row r="80" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C80" s="0"/>
       <c r="E80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B81" s="3"/>
+      <c r="A81" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C81" s="0"/>
       <c r="D81" s="3"/>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
+    <row r="82" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="0"/>
       <c r="E82" s="3"/>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
+    <row r="83" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="0"/>
       <c r="D83" s="3"/>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
+    <row r="84" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C84" s="0"/>
       <c r="E84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="D86" s="5"/>
     </row>
     <row r="87" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="D88" s="5"/>
     </row>
     <row r="89" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="D90" s="5"/>
     </row>
     <row r="91" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="5"/>
@@ -1790,31 +1936,31 @@
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="E92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="D93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -1822,35 +1968,35 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="8" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="8" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="D97" s="5"/>
     </row>
     <row r="98" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>